<commit_message>
separate clr and pending bit, align doc
</commit_message>
<xml_diff>
--- a/doc/I2S_reference.xlsx
+++ b/doc/I2S_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -1126,7 +1126,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1154,33 +1154,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1264,35 +1248,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1344,15 +1328,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1360,7 +1340,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1372,71 +1352,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1452,15 +1416,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1468,10 +1432,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1484,35 +1444,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1584,16 +1528,16 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.2040816326531"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +1815,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1886,17 +1830,17 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="29" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="29" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="29" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="29" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,20 +1989,20 @@
       <c r="A14" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="43" t="s">
         <v>70</v>
       </c>
       <c r="D15" s="29" t="s">
@@ -2067,10 +2011,10 @@
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -2079,105 +2023,105 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="44" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="46" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="46" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47" t="s">
+      <c r="A26" s="45"/>
+      <c r="B26" s="46" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="46" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47" t="s">
+      <c r="A29" s="45"/>
+      <c r="B29" s="46" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="46" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="46" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47" t="s">
+      <c r="A32" s="45"/>
+      <c r="B32" s="46" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="46" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2185,47 +2129,47 @@
       <c r="A34" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="42"/>
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="42"/>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="44" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="48"/>
-      <c r="B38" s="47" t="s">
+      <c r="A38" s="47"/>
+      <c r="B38" s="46" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="49"/>
-      <c r="B40" s="45" t="s">
+      <c r="A40" s="48"/>
+      <c r="B40" s="44" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2239,7 +2183,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2254,73 +2198,73 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="50" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="50" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="50" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="29" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="45.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="49" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="49" width="24.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="49" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="29" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="49" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2335,23 +2279,23 @@
   </sheetPr>
   <dimension ref="A1:AMC57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="29" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="29" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="29" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="29" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1017" min="23" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="29" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="29" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="29" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="29" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="23" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,34 +2310,34 @@
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="49" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="53" t="s">
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="49" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AC1" s="49"/>
+      <c r="AC1" s="48"/>
       <c r="AD1" s="0"/>
       <c r="AE1" s="0"/>
       <c r="AF1" s="0"/>
@@ -3383,92 +3327,92 @@
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
     </row>
-    <row r="2" s="59" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+    <row r="2" s="58" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="57" t="s">
+      <c r="O2" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="P2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="R2" s="57" t="s">
+      <c r="R2" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="57" t="s">
+      <c r="T2" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="57" t="s">
+      <c r="U2" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="V2" s="57" t="s">
+      <c r="V2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="56" t="s">
+      <c r="Y2" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" s="57" t="s">
+      <c r="AA2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="56" t="s">
+      <c r="AB2" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="AC2" s="58" t="s">
+      <c r="AC2" s="57" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3476,10 +3420,10 @@
       <c r="A3" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3487,10 +3431,10 @@
       <c r="A4" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3498,10 +3442,10 @@
       <c r="A5" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3509,10 +3453,10 @@
       <c r="A6" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3520,10 +3464,10 @@
       <c r="A7" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3531,10 +3475,10 @@
       <c r="A8" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3542,10 +3486,10 @@
       <c r="A9" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3553,10 +3497,10 @@
       <c r="A10" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3564,10 +3508,10 @@
       <c r="A11" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3575,362 +3519,362 @@
       <c r="A12" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="59" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="61" t="s">
+      <c r="C33" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="59" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="61" t="s">
+      <c r="C35" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="60" t="s">
+      <c r="A38" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="61" t="s">
+      <c r="C43" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="61" t="s">
+      <c r="C44" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3938,10 +3882,10 @@
       <c r="A45" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3949,10 +3893,10 @@
       <c r="A46" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3960,10 +3904,10 @@
       <c r="A47" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="61" t="s">
+      <c r="C47" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3971,10 +3915,10 @@
       <c r="A48" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="61" t="s">
+      <c r="C48" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3982,10 +3926,10 @@
       <c r="A49" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="61" t="s">
+      <c r="C49" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3993,10 +3937,10 @@
       <c r="A50" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="61" t="s">
+      <c r="C50" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4004,10 +3948,10 @@
       <c r="A51" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="61" t="s">
+      <c r="C51" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4015,10 +3959,10 @@
       <c r="A52" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="61" t="s">
+      <c r="B52" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4026,10 +3970,10 @@
       <c r="A53" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="61" t="s">
+      <c r="C53" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4037,10 +3981,10 @@
       <c r="A54" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4048,10 +3992,10 @@
       <c r="A55" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="61" t="s">
+      <c r="C55" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4059,10 +4003,10 @@
       <c r="A56" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="61" t="s">
+      <c r="C56" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4070,10 +4014,10 @@
       <c r="A57" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="61" t="s">
+      <c r="B57" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4113,7 +4057,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4128,80 +4072,80 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="65" width="19.3061224489796"/>
-    <col collapsed="false" hidden="true" max="2" min="2" style="65" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="66" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="65" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="66" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="30" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="65" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="65" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="65" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="60" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="61" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="60" width="4.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="61" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="60" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="60" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="60" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="62" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="65" t="n">
+      <c r="D2" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="66" t="s">
+      <c r="F2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I2" s="30" t="s">
@@ -4210,25 +4154,25 @@
       <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="65" t="n">
+      <c r="D3" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="66" t="s">
+      <c r="F3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I3" s="30" t="s">
@@ -4237,25 +4181,25 @@
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="65" t="n">
+      <c r="D4" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="66" t="s">
+      <c r="F4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="61" t="s">
         <v>179</v>
       </c>
       <c r="I4" s="30" t="s">
@@ -4264,52 +4208,52 @@
       <c r="J4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="66" t="s">
+      <c r="D5" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="E5" s="66" t="s">
+      <c r="E5" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="61" t="s">
         <v>186</v>
       </c>
       <c r="I5" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="66"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="61" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="65" t="n">
+      <c r="D6" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" s="66" t="s">
+      <c r="F6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I6" s="30" t="s">
@@ -4318,25 +4262,25 @@
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="65" t="n">
+      <c r="D7" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="66" t="s">
+      <c r="F7" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I7" s="30" t="s">
@@ -4345,25 +4289,25 @@
       <c r="J7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="65" t="n">
+      <c r="D8" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="66" t="s">
+      <c r="F8" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="61" t="s">
         <v>179</v>
       </c>
       <c r="I8" s="30" t="s">
@@ -4372,52 +4316,52 @@
       <c r="J8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="F9" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="61" t="s">
         <v>186</v>
       </c>
       <c r="I9" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="J9" s="66"/>
+      <c r="J9" s="61"/>
     </row>
     <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="60" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="65" t="n">
+      <c r="D10" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="66" t="s">
+      <c r="F10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I10" s="30" t="s">
@@ -4425,25 +4369,25 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="60" t="s">
         <v>201</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="61" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="65" t="n">
+      <c r="D11" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="66" t="s">
+      <c r="F11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I11" s="30" t="s">
@@ -4451,25 +4395,25 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="60" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="D12" s="65" t="n">
+      <c r="D12" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E12" s="66" t="s">
+      <c r="E12" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="66" t="s">
+      <c r="F12" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I12" s="30" t="s">
@@ -4477,25 +4421,25 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="61" t="s">
         <v>208</v>
       </c>
-      <c r="D13" s="65" t="n">
+      <c r="D13" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="66" t="s">
+      <c r="F13" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H13" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I13" s="30" t="s">
@@ -4511,7 +4455,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4526,513 +4470,513 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="70" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="50" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="71" width="75.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="72" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="66" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="67" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="68" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="75" t="n">
+      <c r="C2" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="75" t="n">
+      <c r="D2" s="69" t="n">
         <v>16</v>
       </c>
-      <c r="E2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G2" s="76" t="s">
+      <c r="E2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="71" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="75" t="n">
+      <c r="C3" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="75" t="n">
+      <c r="D3" s="69" t="n">
         <v>17</v>
       </c>
-      <c r="E3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F3" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="76" t="s">
+      <c r="E3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="71" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="65" t="s">
         <v>217</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="75" t="n">
+      <c r="C4" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="75" t="n">
+      <c r="D4" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="76" t="s">
+      <c r="E4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="77" t="s">
+      <c r="H4" s="71" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="75" t="n">
+      <c r="C5" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="75" t="n">
+      <c r="D5" s="69" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F5" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="76" t="s">
+      <c r="E5" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="70" t="s">
         <v>220</v>
       </c>
-      <c r="H5" s="77" t="s">
+      <c r="H5" s="71" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="75" t="n">
+      <c r="C6" s="69" t="n">
         <v>4</v>
       </c>
-      <c r="D6" s="75" t="n">
+      <c r="D6" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6" s="76" t="s">
+      <c r="E6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="77" t="s">
+      <c r="H6" s="71" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="75" t="n">
+      <c r="C7" s="69" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="71" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="75" t="n">
+      <c r="D8" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E8" s="61" t="s">
+        <v>226</v>
+      </c>
+      <c r="F8" s="69" t="s">
         <v>225</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="G8" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="69" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="69" t="n">
+        <v>17</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H12" s="71" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C13" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>220</v>
+      </c>
+      <c r="H13" s="71" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
+        <v>222</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" s="69" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="71" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65" t="s">
+        <v>224</v>
+      </c>
+      <c r="B15" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="69" t="n">
+        <v>6</v>
+      </c>
+      <c r="D15" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G15" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="61" t="s">
         <v>226</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="F16" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="G16" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H7" s="77" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>226</v>
-      </c>
-      <c r="F8" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G8" s="76" t="s">
+      <c r="H16" s="71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>186</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="77" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="H9" s="66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="74" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="75" t="n">
-        <v>16</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F10" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H10" s="77" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="74" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="66" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="75" t="n">
-        <v>17</v>
-      </c>
-      <c r="E11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F11" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" s="77" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="74" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C12" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="77" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="75" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F13" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="74" t="s">
-        <v>222</v>
-      </c>
-      <c r="B14" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="75" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F14" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="77" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F15" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H15" s="77" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="66" t="s">
-        <v>226</v>
-      </c>
-      <c r="F16" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="77" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="D17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="G17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="H17" s="79" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="66" t="s">
+      <c r="H18" s="71" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C18" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="75" t="n">
+      <c r="C19" s="49" t="n">
         <v>8</v>
       </c>
-      <c r="E18" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F18" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G18" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="77" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="70" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="78" t="n">
+      <c r="D19" s="69" t="n">
         <v>8</v>
       </c>
-      <c r="D19" s="75" t="n">
-        <v>8</v>
-      </c>
-      <c r="E19" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="78" t="s">
+      <c r="E19" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="49" t="s">
         <v>174</v>
       </c>
       <c r="H19" s="0" t="s">
@@ -5040,77 +4984,77 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="65" t="s">
         <v>237</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C20" s="78" t="n">
+      <c r="C20" s="49" t="n">
         <v>16</v>
       </c>
-      <c r="D20" s="75" t="n">
+      <c r="D20" s="69" t="n">
         <v>8</v>
       </c>
-      <c r="E20" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="78" t="s">
+      <c r="E20" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="79" t="s">
+      <c r="H20" s="29" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="70" t="s">
+      <c r="A21" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C21" s="78" t="n">
+      <c r="C21" s="49" t="n">
         <v>24</v>
       </c>
-      <c r="D21" s="75" t="n">
+      <c r="D21" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E21" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F21" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="78" t="s">
+      <c r="E21" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H21" s="79" t="s">
+      <c r="H21" s="29" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="65" t="s">
         <v>241</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C22" s="78" t="n">
+      <c r="C22" s="49" t="n">
         <v>25</v>
       </c>
-      <c r="D22" s="75" t="n">
+      <c r="D22" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F22" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="78" t="s">
+      <c r="E22" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="49" t="s">
         <v>174</v>
       </c>
       <c r="H22" s="0" t="s">
@@ -5118,132 +5062,132 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C23" s="78" t="n">
+      <c r="C23" s="49" t="n">
         <v>26</v>
       </c>
-      <c r="D23" s="75" t="n">
+      <c r="D23" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" s="78" t="s">
+      <c r="E23" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="29" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="65" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C24" s="78" t="n">
+      <c r="C24" s="49" t="n">
         <v>28</v>
       </c>
-      <c r="D24" s="75" t="n">
+      <c r="D24" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E24" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G24" s="78" t="s">
+      <c r="E24" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H24" s="79" t="s">
+      <c r="H24" s="29" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C25" s="78" t="n">
+      <c r="C25" s="49" t="n">
         <v>29</v>
       </c>
-      <c r="D25" s="75" t="n">
+      <c r="D25" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E25" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="78" t="s">
+      <c r="E25" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H25" s="80" t="s">
+      <c r="H25" s="60" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="65" t="s">
         <v>249</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C26" s="78" t="n">
+      <c r="C26" s="49" t="n">
         <v>30</v>
       </c>
-      <c r="D26" s="75" t="n">
+      <c r="D26" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E26" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G26" s="78" t="s">
+      <c r="E26" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H26" s="79" t="s">
+      <c r="H26" s="29" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="65" t="s">
         <v>251</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C27" s="78" t="n">
+      <c r="C27" s="49" t="n">
         <v>31</v>
       </c>
-      <c r="D27" s="75" t="n">
+      <c r="D27" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E27" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G27" s="78" t="s">
+      <c r="E27" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="80" t="s">
+      <c r="H27" s="60" t="s">
         <v>252</v>
       </c>
     </row>
@@ -5251,129 +5195,129 @@
       <c r="A28" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="C28" s="50" t="n">
+      <c r="C28" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="D28" s="75" t="n">
+      <c r="D28" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="E28" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F28" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G28" s="78" t="s">
+      <c r="E28" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H28" s="65" t="s">
+      <c r="H28" s="60" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="65" t="s">
         <v>255</v>
       </c>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="C29" s="78" t="n">
+      <c r="C29" s="49" t="n">
         <v>8</v>
       </c>
-      <c r="D29" s="75" t="n">
+      <c r="D29" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="E29" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F29" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="78" t="s">
+      <c r="E29" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H29" s="79" t="s">
+      <c r="H29" s="29" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="65" t="s">
         <v>257</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="78" t="n">
+      <c r="C30" s="49" t="n">
         <v>16</v>
       </c>
-      <c r="D30" s="75" t="n">
+      <c r="D30" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E30" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="78" t="s">
+      <c r="E30" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="79" t="s">
+      <c r="H30" s="29" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="65" t="s">
         <v>259</v>
       </c>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="C31" s="78" t="n">
+      <c r="C31" s="49" t="n">
         <v>17</v>
       </c>
-      <c r="D31" s="75" t="n">
+      <c r="D31" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E31" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F31" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G31" s="78" t="s">
+      <c r="E31" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H31" s="79" t="s">
+      <c r="H31" s="29" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="65" t="s">
         <v>261</v>
       </c>
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="61" t="s">
         <v>201</v>
       </c>
-      <c r="C32" s="78" t="n">
+      <c r="C32" s="49" t="n">
         <v>31</v>
       </c>
-      <c r="D32" s="75" t="n">
+      <c r="D32" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E32" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G32" s="78" t="s">
+      <c r="E32" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H32" s="79" t="s">
+      <c r="H32" s="29" t="s">
         <v>262</v>
       </c>
     </row>
@@ -5381,236 +5325,236 @@
       <c r="A33" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C33" s="50" t="n">
+      <c r="C33" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="75" t="n">
+      <c r="D33" s="69" t="n">
         <v>3</v>
       </c>
-      <c r="E33" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="78" t="s">
+      <c r="E33" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H33" s="65" t="s">
+      <c r="H33" s="60" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="70" t="s">
+      <c r="A34" s="65" t="s">
         <v>264</v>
       </c>
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C34" s="78" t="n">
+      <c r="C34" s="49" t="n">
         <v>8</v>
       </c>
-      <c r="D34" s="75" t="n">
+      <c r="D34" s="69" t="n">
         <v>5</v>
       </c>
-      <c r="E34" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F34" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G34" s="78" t="s">
+      <c r="E34" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H34" s="79" t="s">
+      <c r="H34" s="29" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="65" t="s">
         <v>265</v>
       </c>
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="78" t="n">
+      <c r="C35" s="49" t="n">
         <v>16</v>
       </c>
-      <c r="D35" s="75" t="n">
+      <c r="D35" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E35" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F35" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G35" s="78" t="s">
+      <c r="E35" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H35" s="79" t="s">
+      <c r="H35" s="29" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="65" t="s">
         <v>266</v>
       </c>
-      <c r="B36" s="66" t="s">
+      <c r="B36" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C36" s="78" t="n">
+      <c r="C36" s="49" t="n">
         <v>17</v>
       </c>
-      <c r="D36" s="75" t="n">
+      <c r="D36" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E36" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F36" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36" s="78" t="s">
+      <c r="E36" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H36" s="79" t="s">
+      <c r="H36" s="29" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="61" t="s">
         <v>204</v>
       </c>
-      <c r="C37" s="78" t="n">
+      <c r="C37" s="49" t="n">
         <v>31</v>
       </c>
-      <c r="D37" s="75" t="n">
+      <c r="D37" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E37" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G37" s="78" t="s">
+      <c r="E37" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H37" s="79" t="s">
+      <c r="H37" s="29" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="70" t="s">
+      <c r="A38" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="B38" s="66" t="s">
+      <c r="B38" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="C38" s="50" t="n">
+      <c r="C38" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="50" t="n">
+      <c r="D38" s="49" t="n">
         <v>3</v>
       </c>
-      <c r="E38" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G38" s="78" t="s">
+      <c r="E38" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F38" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H38" s="70" t="s">
+      <c r="H38" s="65" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="70" t="s">
+      <c r="A39" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="C39" s="50" t="n">
+      <c r="C39" s="49" t="n">
         <v>3</v>
       </c>
-      <c r="D39" s="50" t="n">
+      <c r="D39" s="49" t="n">
         <v>10</v>
       </c>
-      <c r="E39" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="78" t="s">
+      <c r="E39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H39" s="70" t="s">
+      <c r="H39" s="65" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="70" t="s">
+      <c r="A40" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="C40" s="50" t="n">
+      <c r="C40" s="49" t="n">
         <v>13</v>
       </c>
-      <c r="D40" s="50" t="n">
+      <c r="D40" s="49" t="n">
         <v>2</v>
       </c>
-      <c r="E40" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" s="78" t="s">
+      <c r="E40" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F40" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H40" s="70"/>
+      <c r="H40" s="65"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="B41" s="66" t="s">
+      <c r="B41" s="61" t="s">
         <v>207</v>
       </c>
-      <c r="C41" s="50" t="n">
+      <c r="C41" s="49" t="n">
         <v>31</v>
       </c>
-      <c r="D41" s="50" t="n">
+      <c r="D41" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="E41" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G41" s="78" t="s">
+      <c r="E41" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H41" s="70"/>
+      <c r="H41" s="65"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5625,55 +5569,55 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="72" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="72" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="50" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="71" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="72" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="67" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="67" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="66" width="31.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="67" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="72" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5688,33 +5632,33 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="75" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="69" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="72" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>276</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="72" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5729,45 +5673,45 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="70" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="79.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="72" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Remove empty rows containing -
</commit_message>
<xml_diff>
--- a/doc/I2S_reference.xlsx
+++ b/doc/I2S_reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Info " sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="272">
   <si>
     <t xml:space="preserve">Document Information</t>
   </si>
@@ -628,15 +628,6 @@
     <t xml:space="preserve">RX Channel 0 I2S uDMA transfer configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">I2S_RX_INITCFG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0xC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
     <t xml:space="preserve">I2S_TX_SADDR</t>
   </si>
   <si>
@@ -662,12 +653,6 @@
   </si>
   <si>
     <t xml:space="preserve"> TX Channel I2S uDMA transfer configuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2S_TX_INITCFG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0x1C</t>
   </si>
   <si>
     <t xml:space="preserve">I2S_CLKCFG_SETUP</t>
@@ -788,9 +773,6 @@
   </si>
   <si>
     <t xml:space="preserve">TX_SIZE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESERVED</t>
   </si>
   <si>
     <t xml:space="preserve">MASTER_CLK_DIV</t>
@@ -1126,7 +1108,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1154,33 +1136,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="73">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1264,35 +1230,35 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1344,15 +1310,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1360,7 +1322,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1372,71 +1334,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1452,15 +1398,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1468,10 +1414,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1484,35 +1426,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in TableStyleLight1" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1584,16 +1510,16 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="11.2040816326531"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="40.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +1797,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1886,17 +1812,17 @@
   </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="29" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="29" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="29" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="29" width="42.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="29" width="29.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="29" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,20 +1971,20 @@
       <c r="A14" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>68</v>
       </c>
       <c r="D14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="43" t="s">
         <v>70</v>
       </c>
       <c r="D15" s="29" t="s">
@@ -2067,10 +1993,10 @@
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="43" t="s">
         <v>73</v>
       </c>
       <c r="D16" s="29" t="s">
@@ -2079,105 +2005,105 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="44" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="44" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="44" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="44" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="44" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="46" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47" t="s">
+      <c r="A24" s="45"/>
+      <c r="B24" s="46" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="45"/>
+      <c r="B25" s="46" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47" t="s">
+      <c r="A26" s="45"/>
+      <c r="B26" s="46" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="45"/>
+      <c r="B27" s="46" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47" t="s">
+      <c r="A28" s="45"/>
+      <c r="B28" s="46" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="46"/>
-      <c r="B29" s="47" t="s">
+      <c r="A29" s="45"/>
+      <c r="B29" s="46" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47" t="s">
+      <c r="A30" s="45"/>
+      <c r="B30" s="46" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46"/>
-      <c r="B31" s="47" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="46" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47" t="s">
+      <c r="A32" s="45"/>
+      <c r="B32" s="46" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="46" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2185,47 +2111,47 @@
       <c r="A34" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="42"/>
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="44" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="42"/>
-      <c r="B36" s="45" t="s">
+      <c r="B36" s="44" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="46" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="48"/>
-      <c r="B38" s="47" t="s">
+      <c r="A38" s="47"/>
+      <c r="B38" s="46" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="49" t="s">
+      <c r="A39" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="B39" s="45" t="s">
+      <c r="B39" s="44" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="49"/>
-      <c r="B40" s="45" t="s">
+      <c r="A40" s="48"/>
+      <c r="B40" s="44" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2239,7 +2165,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2254,73 +2180,73 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="50" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="45.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="50" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="50" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="50" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="29" width="10.3928571428571"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="49" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="45.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="49" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="49" width="24.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="49" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="29" width="10.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="50" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="49" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2335,23 +2261,23 @@
   </sheetPr>
   <dimension ref="A1:AMC57"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="29" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="29" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="29" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="29" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="16" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="29" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1017" min="23" style="29" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="1018" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="29" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="29" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="29" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="29" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="16" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="29" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="23" style="29" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1018" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,34 +2292,34 @@
       <c r="G1" s="42"/>
       <c r="H1" s="42"/>
       <c r="I1" s="42"/>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="49" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="53" t="s">
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="49" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="AC1" s="49"/>
+      <c r="AC1" s="48"/>
       <c r="AD1" s="0"/>
       <c r="AE1" s="0"/>
       <c r="AF1" s="0"/>
@@ -3383,92 +3309,92 @@
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
     </row>
-    <row r="2" s="59" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="54" t="s">
+    <row r="2" s="58" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="56" t="s">
+      <c r="G2" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L2" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="M2" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="57" t="s">
+      <c r="O2" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="57" t="s">
+      <c r="P2" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="R2" s="57" t="s">
+      <c r="R2" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="S2" s="57" t="s">
+      <c r="S2" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="T2" s="57" t="s">
+      <c r="T2" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="57" t="s">
+      <c r="U2" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="V2" s="57" t="s">
+      <c r="V2" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="W2" s="56" t="s">
+      <c r="W2" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="X2" s="56" t="s">
+      <c r="X2" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="56" t="s">
+      <c r="Y2" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" s="57" t="s">
+      <c r="AA2" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="AB2" s="56" t="s">
+      <c r="AB2" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="AC2" s="58" t="s">
+      <c r="AC2" s="57" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3476,10 +3402,10 @@
       <c r="A3" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3487,10 +3413,10 @@
       <c r="A4" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3498,10 +3424,10 @@
       <c r="A5" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3509,10 +3435,10 @@
       <c r="A6" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3520,10 +3446,10 @@
       <c r="A7" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C7" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3531,10 +3457,10 @@
       <c r="A8" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3542,10 +3468,10 @@
       <c r="A9" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3553,10 +3479,10 @@
       <c r="A10" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3564,10 +3490,10 @@
       <c r="A11" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3575,362 +3501,362 @@
       <c r="A12" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60" t="s">
+      <c r="A13" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60" t="s">
+      <c r="A14" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="61" t="s">
+      <c r="C22" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="60" t="s">
+      <c r="A24" s="29" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="62" t="s">
+      <c r="A25" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="64" t="s">
+      <c r="C25" s="59" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="60" t="s">
+      <c r="A27" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="61" t="s">
+      <c r="B27" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="60" t="s">
+      <c r="A28" s="29" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="61" t="s">
+      <c r="B28" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="60" t="s">
+      <c r="A29" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="61" t="s">
+      <c r="C30" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="60" t="s">
+      <c r="A31" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="60" t="s">
+      <c r="A32" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="B32" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="61" t="s">
+      <c r="C32" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="60" t="s">
+      <c r="A33" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="61" t="s">
+      <c r="C33" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="B34" s="61" t="s">
+      <c r="B34" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="59" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="60" t="s">
+      <c r="A35" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="61" t="s">
+      <c r="B35" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="61" t="s">
+      <c r="C35" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="60" t="s">
+      <c r="A36" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="61" t="s">
+      <c r="B36" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="60" t="s">
+      <c r="A37" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="50" t="s">
+      <c r="B37" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="60" t="s">
+      <c r="A38" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B38" s="50" t="s">
+      <c r="B38" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="60" t="s">
+      <c r="A39" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="61" t="s">
+      <c r="B39" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="60" t="s">
+      <c r="A41" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="60" t="s">
+      <c r="A42" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="61" t="s">
+      <c r="C42" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="60" t="s">
+      <c r="A43" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="61" t="s">
+      <c r="B43" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="61" t="s">
+      <c r="C43" s="49" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="60" t="s">
+      <c r="A44" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="50" t="s">
+      <c r="B44" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C44" s="61" t="s">
+      <c r="C44" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3938,10 +3864,10 @@
       <c r="A45" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3949,10 +3875,10 @@
       <c r="A46" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B46" s="50" t="s">
+      <c r="B46" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="61" t="s">
+      <c r="C46" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3960,10 +3886,10 @@
       <c r="A47" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C47" s="61" t="s">
+      <c r="C47" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3971,10 +3897,10 @@
       <c r="A48" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B48" s="61" t="s">
+      <c r="B48" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C48" s="61" t="s">
+      <c r="C48" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3982,10 +3908,10 @@
       <c r="A49" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="61" t="s">
+      <c r="C49" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -3993,10 +3919,10 @@
       <c r="A50" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="61" t="s">
+      <c r="C50" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4004,10 +3930,10 @@
       <c r="A51" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B51" s="50" t="s">
+      <c r="B51" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="61" t="s">
+      <c r="C51" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4015,10 +3941,10 @@
       <c r="A52" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="61" t="s">
+      <c r="B52" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="61" t="s">
+      <c r="C52" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4026,10 +3952,10 @@
       <c r="A53" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="61" t="s">
+      <c r="C53" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4037,10 +3963,10 @@
       <c r="A54" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C54" s="61" t="s">
+      <c r="C54" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4048,10 +3974,10 @@
       <c r="A55" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="B55" s="50" t="s">
+      <c r="B55" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="61" t="s">
+      <c r="C55" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4059,10 +3985,10 @@
       <c r="A56" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="50" t="s">
+      <c r="B56" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="61" t="s">
+      <c r="C56" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4070,10 +3996,10 @@
       <c r="A57" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="61" t="s">
+      <c r="B57" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="61" t="s">
+      <c r="C57" s="49" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4113,7 +4039,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4126,82 +4052,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="65" width="19.3061224489796"/>
-    <col collapsed="false" hidden="true" max="2" min="2" style="65" width="0"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="66" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="65" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="66" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="30" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="65" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="65" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="65" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="60" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="61" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="60" width="4.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="61" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="30" width="41.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="60" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="60" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="60" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="63" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="62" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="62" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="65" t="n">
+      <c r="D2" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H2" s="66" t="s">
+      <c r="F2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I2" s="30" t="s">
@@ -4210,25 +4136,25 @@
       <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="60" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="66" t="s">
+      <c r="C3" s="61" t="s">
         <v>179</v>
       </c>
-      <c r="D3" s="65" t="n">
+      <c r="D3" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E3" s="66" t="s">
+      <c r="E3" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H3" s="66" t="s">
+      <c r="F3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I3" s="30" t="s">
@@ -4237,25 +4163,25 @@
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="65" t="n">
+      <c r="D4" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="E4" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H4" s="66" t="s">
+      <c r="F4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="61" t="s">
         <v>179</v>
       </c>
       <c r="I4" s="30" t="s">
@@ -4263,53 +4189,53 @@
       </c>
       <c r="J4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="65" t="s">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="D5" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>186</v>
+      <c r="D5" s="60" t="n">
+        <v>32</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="61" t="s">
+        <v>174</v>
       </c>
       <c r="I5" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="J5" s="66"/>
-    </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="65" t="s">
+      <c r="J5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="60" t="s">
         <v>187</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="61" t="s">
         <v>188</v>
       </c>
-      <c r="D6" s="65" t="n">
+      <c r="D6" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E6" s="66" t="s">
+      <c r="E6" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H6" s="66" t="s">
+      <c r="F6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H6" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I6" s="30" t="s">
@@ -4318,190 +4244,138 @@
       <c r="J6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="D7" s="65" t="n">
+      <c r="D7" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H7" s="66" t="s">
-        <v>174</v>
+      <c r="F7" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="61" t="s">
+        <v>179</v>
       </c>
       <c r="I7" s="30" t="s">
         <v>192</v>
       </c>
       <c r="J7" s="0"/>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="65" t="s">
+    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="60" t="s">
         <v>193</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="D8" s="65" t="n">
+      <c r="D8" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="E8" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G8" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H8" s="66" t="s">
-        <v>179</v>
+      <c r="F8" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="61" t="s">
+        <v>174</v>
       </c>
       <c r="I8" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="J8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="65" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="60" t="s">
         <v>196</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="61" t="s">
         <v>197</v>
       </c>
-      <c r="D9" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="H9" s="66" t="s">
-        <v>186</v>
+      <c r="D9" s="60" t="n">
+        <v>32</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H9" s="61" t="s">
+        <v>174</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="J9" s="66"/>
-    </row>
-    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="65" t="s">
         <v>198</v>
       </c>
-      <c r="C10" s="66" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="60" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="65" t="n">
+      <c r="C10" s="61" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H10" s="66" t="s">
+      <c r="F10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H10" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="65" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="66" t="s">
+      <c r="A11" s="60" t="s">
         <v>202</v>
       </c>
-      <c r="D11" s="65" t="n">
+      <c r="C11" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="D11" s="60" t="n">
         <v>32</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="61" t="s">
         <v>175</v>
       </c>
-      <c r="F11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H11" s="66" t="s">
+      <c r="F11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" s="61" t="s">
         <v>174</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="66" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" s="65" t="n">
-        <v>32</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>175</v>
-      </c>
-      <c r="F12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="66" t="s">
-        <v>174</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="65" t="s">
-        <v>207</v>
-      </c>
-      <c r="C13" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="D13" s="65" t="n">
-        <v>32</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>175</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="H13" s="66" t="s">
-        <v>174</v>
-      </c>
-      <c r="I13" s="30" t="s">
-        <v>209</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1" type="list">
@@ -4511,7 +4385,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4524,1093 +4398,1041 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H41" activeCellId="0" sqref="H41"/>
+      <selection pane="bottomLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="70" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="50" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="71" width="75.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="72" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="25.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="16.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="66" width="75.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="67" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="68" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="69" t="n">
+        <v>16</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" s="71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B3" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="C3" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="69" t="n">
+        <v>17</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="71" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="51" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="73" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="74" t="s">
+      <c r="B4" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H4" s="71" t="s">
         <v>213</v>
       </c>
-      <c r="B2" s="66" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="75" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="65" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="H5" s="71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="69" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H6" s="71" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="B7" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>221</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" s="71" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="B8" s="61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H8" s="71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="65" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="61" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="69" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="75" t="n">
+      <c r="D9" s="69" t="n">
         <v>16</v>
       </c>
-      <c r="E2" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F2" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G2" s="76" t="s">
+      <c r="E9" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H9" s="71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" s="61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="69" t="n">
+        <v>17</v>
+      </c>
+      <c r="E10" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H10" s="71" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="65" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H11" s="71" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="65" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="B12" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C12" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="69" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="70" t="s">
         <v>215</v>
       </c>
-      <c r="B3" s="66" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="75" t="n">
+      <c r="H12" s="71" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C13" s="69" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G13" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H13" s="71" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="65" t="s">
+        <v>219</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="71" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="B15" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>220</v>
+      </c>
+      <c r="G15" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="65" t="s">
+        <v>227</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="75" t="n">
+      <c r="D16" s="69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E16" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G16" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="71" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="65" t="s">
+        <v>229</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D17" s="69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="65" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="49" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" s="69" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="B19" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="49" t="n">
+        <v>24</v>
+      </c>
+      <c r="D19" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="65" t="s">
+        <v>235</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="49" t="n">
+        <v>25</v>
+      </c>
+      <c r="D20" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="65" t="s">
+        <v>237</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="49" t="n">
+        <v>26</v>
+      </c>
+      <c r="D21" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="65" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="49" t="n">
+        <v>28</v>
+      </c>
+      <c r="D22" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="65" t="s">
+        <v>241</v>
+      </c>
+      <c r="B23" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C23" s="49" t="n">
+        <v>29</v>
+      </c>
+      <c r="D23" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F23" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G23" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="60" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="B24" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C24" s="49" t="n">
+        <v>30</v>
+      </c>
+      <c r="D24" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F24" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="B25" s="61" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" s="49" t="n">
+        <v>31</v>
+      </c>
+      <c r="D25" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F25" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G25" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="69" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F26" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H26" s="60" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="65" t="s">
+        <v>249</v>
+      </c>
+      <c r="B27" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C27" s="49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D27" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="65" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="49" t="n">
+        <v>16</v>
+      </c>
+      <c r="D28" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="65" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="49" t="n">
         <v>17</v>
       </c>
-      <c r="E3" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F3" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="76" t="s">
+      <c r="D29" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F29" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H3" s="77" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="74" t="s">
-        <v>217</v>
-      </c>
-      <c r="B4" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="75" t="n">
+      <c r="H29" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="65" t="s">
+        <v>255</v>
+      </c>
+      <c r="B30" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="49" t="n">
+        <v>31</v>
+      </c>
+      <c r="D30" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B31" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C31" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="75" t="n">
+      <c r="D31" s="69" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F31" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H31" s="60" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="65" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="49" t="n">
+        <v>8</v>
+      </c>
+      <c r="D32" s="69" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F32" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="65" t="s">
+        <v>259</v>
+      </c>
+      <c r="B33" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C33" s="49" t="n">
+        <v>16</v>
+      </c>
+      <c r="D33" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F4" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="76" t="s">
+      <c r="E33" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G33" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H4" s="77" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="76.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="B5" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" s="75" t="n">
+      <c r="H33" s="29" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="65" t="s">
+        <v>260</v>
+      </c>
+      <c r="B34" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" s="49" t="n">
+        <v>17</v>
+      </c>
+      <c r="D34" s="69" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="75" t="n">
+      <c r="E34" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="B35" s="61" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" s="49" t="n">
+        <v>31</v>
+      </c>
+      <c r="D35" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F35" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="65" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" s="49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H36" s="65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="65" t="s">
+        <v>265</v>
+      </c>
+      <c r="B37" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="49" t="n">
+        <v>3</v>
+      </c>
+      <c r="D37" s="49" t="n">
+        <v>10</v>
+      </c>
+      <c r="E37" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F37" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H37" s="65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="65" t="s">
+        <v>267</v>
+      </c>
+      <c r="B38" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C38" s="49" t="n">
+        <v>13</v>
+      </c>
+      <c r="D38" s="49" t="n">
         <v>2</v>
       </c>
-      <c r="E5" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F5" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="H5" s="77" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
-        <v>222</v>
-      </c>
-      <c r="B6" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C6" s="75" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="75" t="n">
+      <c r="E38" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F38" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="H38" s="65"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="65" t="s">
+        <v>268</v>
+      </c>
+      <c r="B39" s="61" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="49" t="n">
+        <v>31</v>
+      </c>
+      <c r="D39" s="49" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G6" s="76" t="s">
+      <c r="E39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="49" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="77" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C7" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="66" t="s">
-        <v>225</v>
-      </c>
-      <c r="F7" s="75" t="s">
-        <v>226</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" s="77" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="B8" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="C8" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>226</v>
-      </c>
-      <c r="F8" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G8" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H8" s="77" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="66" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="F9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="G9" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="H9" s="66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="74" t="s">
-        <v>230</v>
-      </c>
-      <c r="B10" s="66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="75" t="n">
-        <v>16</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F10" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H10" s="77" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="74" t="s">
-        <v>231</v>
-      </c>
-      <c r="B11" s="66" t="s">
-        <v>190</v>
-      </c>
-      <c r="C11" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" s="75" t="n">
-        <v>17</v>
-      </c>
-      <c r="E11" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F11" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G11" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" s="77" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="74" t="s">
-        <v>217</v>
-      </c>
-      <c r="B12" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C12" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F12" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H12" s="77" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="74" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="75" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F13" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="H13" s="77" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="74" t="s">
-        <v>222</v>
-      </c>
-      <c r="B14" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C14" s="75" t="n">
-        <v>4</v>
-      </c>
-      <c r="D14" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F14" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G14" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="77" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="74" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D15" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F15" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H15" s="77" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="74" t="s">
-        <v>228</v>
-      </c>
-      <c r="B16" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" s="66" t="s">
-        <v>226</v>
-      </c>
-      <c r="F16" s="75" t="s">
-        <v>225</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="77" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="20.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="B17" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="D17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="E17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="F17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="G17" s="78" t="s">
-        <v>186</v>
-      </c>
-      <c r="H17" s="79" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="74" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C18" s="78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="75" t="n">
-        <v>8</v>
-      </c>
-      <c r="E18" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F18" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G18" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="77" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="70" t="s">
-        <v>235</v>
-      </c>
-      <c r="B19" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C19" s="78" t="n">
-        <v>8</v>
-      </c>
-      <c r="D19" s="75" t="n">
-        <v>8</v>
-      </c>
-      <c r="E19" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G19" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H19" s="0" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="74" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="78" t="n">
-        <v>16</v>
-      </c>
-      <c r="D20" s="75" t="n">
-        <v>8</v>
-      </c>
-      <c r="E20" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H20" s="79" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="70" t="s">
-        <v>239</v>
-      </c>
-      <c r="B21" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="78" t="n">
-        <v>24</v>
-      </c>
-      <c r="D21" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F21" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G21" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H21" s="79" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="70" t="s">
-        <v>241</v>
-      </c>
-      <c r="B22" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="78" t="n">
-        <v>25</v>
-      </c>
-      <c r="D22" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F22" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G22" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="74" t="s">
-        <v>243</v>
-      </c>
-      <c r="B23" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C23" s="78" t="n">
-        <v>26</v>
-      </c>
-      <c r="D23" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G23" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H23" s="79" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="70" t="s">
-        <v>245</v>
-      </c>
-      <c r="B24" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C24" s="78" t="n">
-        <v>28</v>
-      </c>
-      <c r="D24" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E24" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F24" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G24" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H24" s="79" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="70" t="s">
-        <v>247</v>
-      </c>
-      <c r="B25" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" s="78" t="n">
-        <v>29</v>
-      </c>
-      <c r="D25" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F25" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H25" s="80" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="70" t="s">
-        <v>249</v>
-      </c>
-      <c r="B26" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C26" s="78" t="n">
-        <v>30</v>
-      </c>
-      <c r="D26" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E26" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G26" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H26" s="79" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="74" t="s">
-        <v>251</v>
-      </c>
-      <c r="B27" s="66" t="s">
-        <v>198</v>
-      </c>
-      <c r="C27" s="78" t="n">
-        <v>31</v>
-      </c>
-      <c r="D27" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F27" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G27" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H27" s="80" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="B28" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="75" t="n">
-        <v>3</v>
-      </c>
-      <c r="E28" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F28" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G28" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H28" s="65" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="70" t="s">
-        <v>255</v>
-      </c>
-      <c r="B29" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="C29" s="78" t="n">
-        <v>8</v>
-      </c>
-      <c r="D29" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="E29" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F29" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H29" s="79" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="70" t="s">
-        <v>257</v>
-      </c>
-      <c r="B30" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="C30" s="78" t="n">
-        <v>16</v>
-      </c>
-      <c r="D30" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E30" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F30" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G30" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H30" s="79" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="74" t="s">
-        <v>259</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="C31" s="78" t="n">
-        <v>17</v>
-      </c>
-      <c r="D31" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E31" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F31" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G31" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H31" s="79" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="70" t="s">
-        <v>261</v>
-      </c>
-      <c r="B32" s="66" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" s="78" t="n">
-        <v>31</v>
-      </c>
-      <c r="D32" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G32" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H32" s="79" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="B33" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="C33" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" s="75" t="n">
-        <v>3</v>
-      </c>
-      <c r="E33" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G33" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H33" s="65" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="70" t="s">
-        <v>264</v>
-      </c>
-      <c r="B34" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" s="78" t="n">
-        <v>8</v>
-      </c>
-      <c r="D34" s="75" t="n">
-        <v>5</v>
-      </c>
-      <c r="E34" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F34" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G34" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H34" s="79" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="70" t="s">
-        <v>265</v>
-      </c>
-      <c r="B35" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="C35" s="78" t="n">
-        <v>16</v>
-      </c>
-      <c r="D35" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F35" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G35" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" s="79" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="74" t="s">
-        <v>266</v>
-      </c>
-      <c r="B36" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="C36" s="78" t="n">
-        <v>17</v>
-      </c>
-      <c r="D36" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F36" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G36" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H36" s="79" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="70" t="s">
-        <v>267</v>
-      </c>
-      <c r="B37" s="66" t="s">
-        <v>204</v>
-      </c>
-      <c r="C37" s="78" t="n">
-        <v>31</v>
-      </c>
-      <c r="D37" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F37" s="75" t="s">
-        <v>176</v>
-      </c>
-      <c r="G37" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H37" s="79" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="70" t="s">
-        <v>269</v>
-      </c>
-      <c r="B38" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="C38" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="E38" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F38" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G38" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H38" s="70" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="70" t="s">
-        <v>271</v>
-      </c>
-      <c r="B39" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="C39" s="50" t="n">
-        <v>3</v>
-      </c>
-      <c r="D39" s="50" t="n">
-        <v>10</v>
-      </c>
-      <c r="E39" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F39" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G39" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" s="70" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="70" t="s">
-        <v>273</v>
-      </c>
-      <c r="B40" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="50" t="n">
-        <v>13</v>
-      </c>
-      <c r="D40" s="50" t="n">
-        <v>2</v>
-      </c>
-      <c r="E40" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F40" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G40" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" s="70"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="70" t="s">
-        <v>274</v>
-      </c>
-      <c r="B41" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="C41" s="50" t="n">
-        <v>31</v>
-      </c>
-      <c r="D41" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="F41" s="76" t="s">
-        <v>176</v>
-      </c>
-      <c r="G41" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="H41" s="70"/>
+      <c r="H39" s="65"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5625,55 +5447,55 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="72" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="72" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="50" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="50" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="71" width="31.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="72" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="67" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="67" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="49" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="49" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="66" width="31.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="67" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
-        <v>210</v>
-      </c>
-      <c r="B1" s="81" t="s">
-        <v>211</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="A1" s="72" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="50" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -5688,33 +5510,33 @@
   </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="75" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="69" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="79.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
-        <v>275</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>276</v>
-      </c>
-      <c r="C1" s="81" t="s">
+      <c r="A1" s="72" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="72" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5729,45 +5551,45 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="70" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="50" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="50" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="50" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="50" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="79.6428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.04591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="49" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="49" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="49" width="9.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="49" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="79.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
-        <v>277</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>275</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>212</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="A1" s="68" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="72" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>